<commit_message>
Updating surveyor coloumns and rough methods.
</commit_message>
<xml_diff>
--- a/data/T30R11_data.xlsx
+++ b/data/T30R11_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara Fox\Documents\Kara GLO\RStudio\GLO_sage\Sage_GLO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C930424-F46F-42C5-BCA1-0247CD8A2162}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42890298-CC9E-428D-8903-7CFAE7D468D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5295" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4447" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4780" uniqueCount="275">
   <si>
     <t>Survey_type</t>
   </si>
@@ -1355,8 +1355,8 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="A315" sqref="A315:XFD320"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1466,7 +1466,9 @@
       <c r="I2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L2" s="5" t="s">
         <v>207</v>
       </c>
@@ -1493,7 +1495,9 @@
       <c r="I3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L3" s="5" t="s">
         <v>207</v>
       </c>
@@ -1524,7 +1528,9 @@
       <c r="I4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L4" s="5" t="s">
         <v>207</v>
       </c>
@@ -1551,7 +1557,9 @@
       <c r="I5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L5" s="5" t="s">
         <v>207</v>
       </c>
@@ -1578,7 +1586,9 @@
       <c r="I6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L6" s="5" t="s">
         <v>207</v>
       </c>
@@ -1605,7 +1615,9 @@
       <c r="I7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L7" s="5" t="s">
         <v>207</v>
       </c>
@@ -1632,7 +1644,9 @@
       <c r="I8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L8" s="5" t="s">
         <v>207</v>
       </c>
@@ -1659,7 +1673,9 @@
       <c r="I9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L9" s="5" t="s">
         <v>207</v>
       </c>
@@ -1686,7 +1702,9 @@
       <c r="I10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L10" s="5" t="s">
         <v>207</v>
       </c>
@@ -1713,7 +1731,9 @@
       <c r="I11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L11" s="5" t="s">
         <v>207</v>
       </c>
@@ -1740,7 +1760,9 @@
       <c r="I12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="5"/>
+      <c r="J12" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L12" s="5" t="s">
         <v>207</v>
       </c>
@@ -1767,7 +1789,9 @@
       <c r="I13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L13" s="5" t="s">
         <v>207</v>
       </c>
@@ -1794,7 +1818,9 @@
       <c r="I14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L14" s="5" t="s">
         <v>207</v>
       </c>
@@ -1821,7 +1847,9 @@
       <c r="I15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L15" s="5" t="s">
         <v>207</v>
       </c>
@@ -1848,7 +1876,9 @@
       <c r="I16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L16" s="5" t="s">
         <v>207</v>
       </c>
@@ -1875,7 +1905,9 @@
       <c r="I17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="J17" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L17" s="5" t="s">
         <v>207</v>
       </c>
@@ -1902,7 +1934,9 @@
       <c r="I18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L18" s="5" t="s">
         <v>207</v>
       </c>
@@ -1929,7 +1963,9 @@
       <c r="I19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L19" s="5" t="s">
         <v>207</v>
       </c>
@@ -1956,7 +1992,9 @@
       <c r="I20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L20" s="5" t="s">
         <v>207</v>
       </c>
@@ -1987,7 +2025,9 @@
       <c r="I21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L21" s="5" t="s">
         <v>207</v>
       </c>
@@ -2014,7 +2054,9 @@
       <c r="I22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L22" s="5" t="s">
         <v>207</v>
       </c>
@@ -2041,7 +2083,9 @@
       <c r="I23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="J23" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L23" s="5" t="s">
         <v>207</v>
       </c>
@@ -2068,7 +2112,9 @@
       <c r="I24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="J24" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L24" s="5" t="s">
         <v>207</v>
       </c>
@@ -2099,7 +2145,9 @@
       <c r="I25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="J25" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L25" s="5" t="s">
         <v>207</v>
       </c>
@@ -2126,7 +2174,9 @@
       <c r="I26" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="J26" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L26" s="5" t="s">
         <v>207</v>
       </c>
@@ -2153,7 +2203,9 @@
       <c r="I27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="J27" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L27" s="5" t="s">
         <v>207</v>
       </c>
@@ -2180,7 +2232,9 @@
       <c r="I28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J28" s="5"/>
+      <c r="J28" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L28" s="5" t="s">
         <v>207</v>
       </c>
@@ -2207,7 +2261,9 @@
       <c r="I29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="J29" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L29" s="5" t="s">
         <v>207</v>
       </c>
@@ -2234,7 +2290,9 @@
       <c r="I30" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="J30" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L30" s="5" t="s">
         <v>207</v>
       </c>
@@ -2261,7 +2319,9 @@
       <c r="I31" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="J31" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L31" s="5" t="s">
         <v>207</v>
       </c>
@@ -2288,7 +2348,9 @@
       <c r="I32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J32" s="5"/>
+      <c r="J32" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L32" s="5" t="s">
         <v>207</v>
       </c>
@@ -2315,7 +2377,9 @@
       <c r="I33" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="J33" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L33" s="5" t="s">
         <v>207</v>
       </c>
@@ -2342,7 +2406,9 @@
       <c r="I34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="J34" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L34" s="5" t="s">
         <v>207</v>
       </c>
@@ -2369,7 +2435,9 @@
       <c r="I35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="J35" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L35" s="5" t="s">
         <v>207</v>
       </c>
@@ -2396,7 +2464,9 @@
       <c r="I36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J36" s="5"/>
+      <c r="J36" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L36" s="5" t="s">
         <v>207</v>
       </c>
@@ -2423,7 +2493,9 @@
       <c r="I37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J37" s="5"/>
+      <c r="J37" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L37" s="5" t="s">
         <v>207</v>
       </c>
@@ -2450,7 +2522,9 @@
       <c r="I38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="5"/>
+      <c r="J38" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L38" s="5" t="s">
         <v>207</v>
       </c>
@@ -2477,7 +2551,9 @@
       <c r="I39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J39" s="5"/>
+      <c r="J39" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L39" s="5" t="s">
         <v>207</v>
       </c>
@@ -2504,7 +2580,9 @@
       <c r="I40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="5"/>
+      <c r="J40" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L40" s="5" t="s">
         <v>207</v>
       </c>
@@ -2535,7 +2613,9 @@
       <c r="I41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J41" s="5"/>
+      <c r="J41" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L41" s="5" t="s">
         <v>207</v>
       </c>
@@ -2562,7 +2642,9 @@
       <c r="I42" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J42" s="5"/>
+      <c r="J42" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L42" s="5" t="s">
         <v>207</v>
       </c>
@@ -2589,7 +2671,9 @@
       <c r="I43" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J43" s="5"/>
+      <c r="J43" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L43" s="5" t="s">
         <v>207</v>
       </c>
@@ -2616,7 +2700,9 @@
       <c r="I44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J44" s="5"/>
+      <c r="J44" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L44" s="5" t="s">
         <v>207</v>
       </c>
@@ -2643,7 +2729,9 @@
       <c r="I45" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J45" s="5"/>
+      <c r="J45" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L45" s="5" t="s">
         <v>207</v>
       </c>
@@ -2670,7 +2758,9 @@
       <c r="I46" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J46" s="5"/>
+      <c r="J46" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L46" s="5" t="s">
         <v>207</v>
       </c>
@@ -2697,7 +2787,9 @@
       <c r="I47" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J47" s="5"/>
+      <c r="J47" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L47" s="5" t="s">
         <v>207</v>
       </c>
@@ -2724,7 +2816,9 @@
       <c r="I48" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J48" s="5"/>
+      <c r="J48" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L48" s="5" t="s">
         <v>207</v>
       </c>
@@ -2755,7 +2849,9 @@
       <c r="I49" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J49" s="5"/>
+      <c r="J49" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L49" s="5" t="s">
         <v>207</v>
       </c>
@@ -2782,7 +2878,9 @@
       <c r="I50" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J50" s="5"/>
+      <c r="J50" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L50" s="5" t="s">
         <v>207</v>
       </c>
@@ -2809,7 +2907,9 @@
       <c r="I51" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J51" s="5"/>
+      <c r="J51" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L51" s="5" t="s">
         <v>207</v>
       </c>
@@ -2836,7 +2936,9 @@
       <c r="I52" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J52" s="5"/>
+      <c r="J52" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L52" s="5" t="s">
         <v>207</v>
       </c>
@@ -2863,7 +2965,9 @@
       <c r="I53" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J53" s="5"/>
+      <c r="J53" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L53" s="5" t="s">
         <v>207</v>
       </c>
@@ -2890,7 +2994,9 @@
       <c r="I54" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J54" s="5"/>
+      <c r="J54" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L54" s="5" t="s">
         <v>207</v>
       </c>
@@ -2917,7 +3023,9 @@
       <c r="I55" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J55" s="5"/>
+      <c r="J55" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L55" s="5" t="s">
         <v>207</v>
       </c>
@@ -2944,7 +3052,9 @@
       <c r="I56" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J56" s="5"/>
+      <c r="J56" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L56" s="5" t="s">
         <v>207</v>
       </c>
@@ -2971,7 +3081,9 @@
       <c r="I57" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J57" s="5"/>
+      <c r="J57" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L57" s="5" t="s">
         <v>207</v>
       </c>
@@ -2998,7 +3110,9 @@
       <c r="I58" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J58" s="5"/>
+      <c r="J58" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L58" s="5" t="s">
         <v>207</v>
       </c>
@@ -3025,7 +3139,9 @@
       <c r="I59" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J59" s="5"/>
+      <c r="J59" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L59" s="5" t="s">
         <v>207</v>
       </c>
@@ -3052,7 +3168,9 @@
       <c r="I60" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J60" s="5"/>
+      <c r="J60" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L60" s="5" t="s">
         <v>207</v>
       </c>
@@ -3079,7 +3197,9 @@
       <c r="I61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J61" s="5"/>
+      <c r="J61" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L61" s="5" t="s">
         <v>207</v>
       </c>
@@ -3106,7 +3226,9 @@
       <c r="I62" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J62" s="5"/>
+      <c r="J62" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L62" s="5" t="s">
         <v>207</v>
       </c>
@@ -3133,7 +3255,9 @@
       <c r="I63" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J63" s="5"/>
+      <c r="J63" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L63" s="5" t="s">
         <v>207</v>
       </c>
@@ -3160,7 +3284,9 @@
       <c r="I64" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J64" s="5"/>
+      <c r="J64" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L64" s="5" t="s">
         <v>207</v>
       </c>
@@ -3187,7 +3313,9 @@
       <c r="I65" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J65" s="5"/>
+      <c r="J65" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L65" s="5" t="s">
         <v>207</v>
       </c>
@@ -3214,7 +3342,9 @@
       <c r="I66" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J66" s="5"/>
+      <c r="J66" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L66" s="5" t="s">
         <v>207</v>
       </c>
@@ -3241,7 +3371,9 @@
       <c r="I67" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="5"/>
+      <c r="J67" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L67" s="5" t="s">
         <v>207</v>
       </c>
@@ -3268,7 +3400,9 @@
       <c r="I68" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J68" s="5"/>
+      <c r="J68" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L68" s="5" t="s">
         <v>207</v>
       </c>
@@ -3295,7 +3429,9 @@
       <c r="I69" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J69" s="5"/>
+      <c r="J69" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L69" s="5" t="s">
         <v>207</v>
       </c>
@@ -3322,7 +3458,9 @@
       <c r="I70" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J70" s="5"/>
+      <c r="J70" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L70" s="5" t="s">
         <v>207</v>
       </c>
@@ -3349,7 +3487,9 @@
       <c r="I71" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J71" s="5"/>
+      <c r="J71" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L71" s="5" t="s">
         <v>207</v>
       </c>
@@ -3376,7 +3516,9 @@
       <c r="I72" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J72" s="5"/>
+      <c r="J72" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L72" s="5" t="s">
         <v>207</v>
       </c>
@@ -3407,7 +3549,9 @@
       <c r="I73" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J73" s="5"/>
+      <c r="J73" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L73" s="5" t="s">
         <v>207</v>
       </c>
@@ -3434,7 +3578,9 @@
       <c r="I74" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J74" s="5"/>
+      <c r="J74" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L74" s="5" t="s">
         <v>207</v>
       </c>
@@ -3461,7 +3607,9 @@
       <c r="I75" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J75" s="5"/>
+      <c r="J75" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L75" s="5" t="s">
         <v>207</v>
       </c>
@@ -3488,7 +3636,9 @@
       <c r="I76" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J76" s="5"/>
+      <c r="J76" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L76" s="5" t="s">
         <v>207</v>
       </c>
@@ -3515,7 +3665,9 @@
       <c r="I77" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J77" s="5"/>
+      <c r="J77" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L77" s="5" t="s">
         <v>207</v>
       </c>
@@ -3542,7 +3694,9 @@
       <c r="I78" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J78" s="5"/>
+      <c r="J78" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L78" s="5" t="s">
         <v>207</v>
       </c>
@@ -3569,7 +3723,9 @@
       <c r="I79" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J79" s="5"/>
+      <c r="J79" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L79" s="5" t="s">
         <v>207</v>
       </c>
@@ -3596,7 +3752,9 @@
       <c r="I80" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J80" s="5"/>
+      <c r="J80" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L80" s="5" t="s">
         <v>207</v>
       </c>
@@ -3627,7 +3785,9 @@
       <c r="I81" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J81" s="5"/>
+      <c r="J81" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L81" s="5" t="s">
         <v>207</v>
       </c>
@@ -3654,7 +3814,9 @@
       <c r="I82" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J82" s="5"/>
+      <c r="J82" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L82" s="5" t="s">
         <v>207</v>
       </c>
@@ -3681,7 +3843,9 @@
       <c r="I83" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J83" s="5"/>
+      <c r="J83" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L83" s="5" t="s">
         <v>207</v>
       </c>
@@ -3708,7 +3872,9 @@
       <c r="I84" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J84" s="5"/>
+      <c r="J84" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L84" s="5" t="s">
         <v>207</v>
       </c>
@@ -3735,7 +3901,9 @@
       <c r="I85" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J85" s="5"/>
+      <c r="J85" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L85" s="5" t="s">
         <v>207</v>
       </c>
@@ -3762,7 +3930,9 @@
       <c r="I86" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J86" s="5"/>
+      <c r="J86" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L86" s="5" t="s">
         <v>207</v>
       </c>
@@ -3789,7 +3959,9 @@
       <c r="I87" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J87" s="5"/>
+      <c r="J87" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L87" s="5" t="s">
         <v>207</v>
       </c>
@@ -3816,7 +3988,9 @@
       <c r="I88" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J88" s="5"/>
+      <c r="J88" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L88" s="5" t="s">
         <v>207</v>
       </c>
@@ -3847,7 +4021,9 @@
       <c r="I89" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J89" s="5"/>
+      <c r="J89" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L89" s="5" t="s">
         <v>207</v>
       </c>
@@ -3874,7 +4050,9 @@
       <c r="I90" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J90" s="5"/>
+      <c r="J90" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L90" s="5" t="s">
         <v>207</v>
       </c>
@@ -3901,7 +4079,9 @@
       <c r="I91" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J91" s="5"/>
+      <c r="J91" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L91" s="5" t="s">
         <v>207</v>
       </c>
@@ -3928,7 +4108,9 @@
       <c r="I92" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J92" s="5"/>
+      <c r="J92" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L92" s="5" t="s">
         <v>207</v>
       </c>
@@ -3955,7 +4137,9 @@
       <c r="I93" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J93" s="5"/>
+      <c r="J93" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L93" s="5" t="s">
         <v>207</v>
       </c>
@@ -3982,7 +4166,9 @@
       <c r="I94" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J94" s="5"/>
+      <c r="J94" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L94" s="5" t="s">
         <v>207</v>
       </c>
@@ -4009,7 +4195,9 @@
       <c r="I95" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J95" s="5"/>
+      <c r="J95" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L95" s="5" t="s">
         <v>207</v>
       </c>
@@ -4036,7 +4224,9 @@
       <c r="I96" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J96" s="5"/>
+      <c r="J96" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L96" s="5" t="s">
         <v>207</v>
       </c>
@@ -4063,7 +4253,9 @@
       <c r="I97" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J97" s="5"/>
+      <c r="J97" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L97" s="5" t="s">
         <v>207</v>
       </c>
@@ -4090,7 +4282,9 @@
       <c r="I98" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="J98" s="5"/>
+      <c r="J98" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L98" s="5" t="s">
         <v>207</v>
       </c>
@@ -4117,7 +4311,9 @@
       <c r="I99" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J99" s="5"/>
+      <c r="J99" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L99" s="5" t="s">
         <v>207</v>
       </c>
@@ -4144,7 +4340,9 @@
       <c r="I100" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J100" s="5"/>
+      <c r="J100" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L100" s="5" t="s">
         <v>207</v>
       </c>
@@ -4171,7 +4369,9 @@
       <c r="I101" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J101" s="5"/>
+      <c r="J101" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L101" s="5" t="s">
         <v>207</v>
       </c>
@@ -4198,7 +4398,9 @@
       <c r="I102" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J102" s="5"/>
+      <c r="J102" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L102" s="5" t="s">
         <v>207</v>
       </c>
@@ -4229,7 +4431,9 @@
       <c r="I103" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J103" s="5"/>
+      <c r="J103" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L103" s="5" t="s">
         <v>207</v>
       </c>
@@ -4256,7 +4460,9 @@
       <c r="I104" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J104" s="5"/>
+      <c r="J104" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L104" s="5" t="s">
         <v>207</v>
       </c>
@@ -4283,7 +4489,9 @@
       <c r="I105" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J105" s="5"/>
+      <c r="J105" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L105" s="5" t="s">
         <v>207</v>
       </c>
@@ -4310,7 +4518,9 @@
       <c r="I106" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J106" s="5"/>
+      <c r="J106" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L106" s="5" t="s">
         <v>207</v>
       </c>
@@ -4337,7 +4547,9 @@
       <c r="I107" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J107" s="5"/>
+      <c r="J107" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L107" s="5" t="s">
         <v>207</v>
       </c>
@@ -4364,7 +4576,9 @@
       <c r="I108" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J108" s="5"/>
+      <c r="J108" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L108" s="5" t="s">
         <v>207</v>
       </c>
@@ -4391,7 +4605,9 @@
       <c r="I109" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J109" s="5"/>
+      <c r="J109" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L109" s="5" t="s">
         <v>207</v>
       </c>
@@ -4418,7 +4634,9 @@
       <c r="I110" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J110" s="5"/>
+      <c r="J110" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L110" s="5" t="s">
         <v>207</v>
       </c>
@@ -4445,7 +4663,9 @@
       <c r="I111" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J111" s="5"/>
+      <c r="J111" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L111" s="5" t="s">
         <v>207</v>
       </c>
@@ -4472,7 +4692,9 @@
       <c r="I112" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J112" s="5"/>
+      <c r="J112" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L112" s="5" t="s">
         <v>207</v>
       </c>
@@ -4499,7 +4721,9 @@
       <c r="I113" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J113" s="5"/>
+      <c r="J113" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L113" s="5" t="s">
         <v>207</v>
       </c>
@@ -4526,7 +4750,9 @@
       <c r="I114" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J114" s="5"/>
+      <c r="J114" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L114" s="5" t="s">
         <v>207</v>
       </c>
@@ -4553,7 +4779,9 @@
       <c r="I115" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J115" s="5"/>
+      <c r="J115" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L115" s="5" t="s">
         <v>207</v>
       </c>
@@ -4580,7 +4808,9 @@
       <c r="I116" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J116" s="5"/>
+      <c r="J116" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L116" s="5" t="s">
         <v>207</v>
       </c>
@@ -4607,7 +4837,9 @@
       <c r="I117" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J117" s="5"/>
+      <c r="J117" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L117" s="5" t="s">
         <v>207</v>
       </c>
@@ -4634,7 +4866,9 @@
       <c r="I118" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J118" s="5"/>
+      <c r="J118" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L118" s="5" t="s">
         <v>207</v>
       </c>
@@ -4661,7 +4895,9 @@
       <c r="I119" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J119" s="5"/>
+      <c r="J119" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L119" s="5" t="s">
         <v>207</v>
       </c>
@@ -4688,7 +4924,9 @@
       <c r="I120" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J120" s="5"/>
+      <c r="J120" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L120" s="5" t="s">
         <v>207</v>
       </c>
@@ -4715,7 +4953,9 @@
       <c r="I121" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J121" s="5"/>
+      <c r="J121" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L121" s="5" t="s">
         <v>207</v>
       </c>
@@ -4742,7 +4982,9 @@
       <c r="I122" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J122" s="5"/>
+      <c r="J122" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L122" s="5" t="s">
         <v>207</v>
       </c>
@@ -4769,7 +5011,9 @@
       <c r="I123" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J123" s="5"/>
+      <c r="J123" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L123" s="5" t="s">
         <v>207</v>
       </c>
@@ -4796,7 +5040,9 @@
       <c r="I124" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J124" s="5"/>
+      <c r="J124" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L124" s="5" t="s">
         <v>207</v>
       </c>
@@ -4823,7 +5069,9 @@
       <c r="I125" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="J125" s="5"/>
+      <c r="J125" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L125" s="5" t="s">
         <v>207</v>
       </c>
@@ -4850,7 +5098,9 @@
       <c r="I126" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J126" s="5"/>
+      <c r="J126" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L126" s="5" t="s">
         <v>207</v>
       </c>
@@ -4877,7 +5127,9 @@
       <c r="I127" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J127" s="5"/>
+      <c r="J127" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L127" s="5" t="s">
         <v>207</v>
       </c>
@@ -4904,7 +5156,9 @@
       <c r="I128" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J128" s="5"/>
+      <c r="J128" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L128" s="5" t="s">
         <v>207</v>
       </c>
@@ -4931,7 +5185,9 @@
       <c r="I129" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J129" s="5"/>
+      <c r="J129" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L129" s="5" t="s">
         <v>207</v>
       </c>
@@ -4962,7 +5218,9 @@
       <c r="I130" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J130" s="5"/>
+      <c r="J130" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L130" s="5" t="s">
         <v>207</v>
       </c>
@@ -4989,7 +5247,9 @@
       <c r="I131" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J131" s="5"/>
+      <c r="J131" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L131" s="5" t="s">
         <v>207</v>
       </c>
@@ -5016,7 +5276,9 @@
       <c r="I132" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J132" s="5"/>
+      <c r="J132" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L132" s="5" t="s">
         <v>207</v>
       </c>
@@ -5043,7 +5305,9 @@
       <c r="I133" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J133" s="5"/>
+      <c r="J133" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L133" s="5" t="s">
         <v>207</v>
       </c>
@@ -5074,7 +5338,9 @@
       <c r="I134" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J134" s="5"/>
+      <c r="J134" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L134" s="5" t="s">
         <v>207</v>
       </c>
@@ -5101,7 +5367,9 @@
       <c r="I135" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J135" s="5"/>
+      <c r="J135" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L135" s="5" t="s">
         <v>207</v>
       </c>
@@ -5128,7 +5396,9 @@
       <c r="I136" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J136" s="5"/>
+      <c r="J136" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L136" s="5" t="s">
         <v>207</v>
       </c>
@@ -5155,7 +5425,9 @@
       <c r="I137" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J137" s="5"/>
+      <c r="J137" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L137" s="5" t="s">
         <v>207</v>
       </c>
@@ -5182,7 +5454,9 @@
       <c r="I138" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J138" s="5"/>
+      <c r="J138" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L138" s="5" t="s">
         <v>207</v>
       </c>
@@ -5209,7 +5483,9 @@
       <c r="I139" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J139" s="5"/>
+      <c r="J139" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L139" s="5" t="s">
         <v>207</v>
       </c>
@@ -5236,7 +5512,9 @@
       <c r="I140" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J140" s="5"/>
+      <c r="J140" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L140" s="5" t="s">
         <v>207</v>
       </c>
@@ -5263,7 +5541,9 @@
       <c r="I141" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J141" s="5"/>
+      <c r="J141" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L141" s="5" t="s">
         <v>207</v>
       </c>
@@ -5290,7 +5570,9 @@
       <c r="I142" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J142" s="5"/>
+      <c r="J142" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L142" s="5" t="s">
         <v>207</v>
       </c>
@@ -5317,7 +5599,9 @@
       <c r="I143" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J143" s="5"/>
+      <c r="J143" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L143" s="5" t="s">
         <v>207</v>
       </c>
@@ -5344,7 +5628,9 @@
       <c r="I144" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J144" s="5"/>
+      <c r="J144" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L144" s="5" t="s">
         <v>207</v>
       </c>
@@ -5371,7 +5657,9 @@
       <c r="I145" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J145" s="5"/>
+      <c r="J145" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L145" s="5" t="s">
         <v>207</v>
       </c>
@@ -5398,7 +5686,9 @@
       <c r="I146" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="J146" s="5"/>
+      <c r="J146" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L146" s="5" t="s">
         <v>207</v>
       </c>
@@ -5425,7 +5715,9 @@
       <c r="I147" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J147" s="5"/>
+      <c r="J147" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L147" s="5" t="s">
         <v>207</v>
       </c>
@@ -5452,7 +5744,9 @@
       <c r="I148" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J148" s="5"/>
+      <c r="J148" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L148" s="5" t="s">
         <v>207</v>
       </c>
@@ -5479,7 +5773,9 @@
       <c r="I149" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J149" s="5"/>
+      <c r="J149" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L149" s="5" t="s">
         <v>207</v>
       </c>
@@ -5506,7 +5802,9 @@
       <c r="I150" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J150" s="5"/>
+      <c r="J150" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L150" s="5" t="s">
         <v>207</v>
       </c>
@@ -5533,7 +5831,9 @@
       <c r="I151" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J151" s="5"/>
+      <c r="J151" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L151" s="5" t="s">
         <v>207</v>
       </c>
@@ -5560,7 +5860,9 @@
       <c r="I152" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="J152" s="5"/>
+      <c r="J152" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L152" s="5" t="s">
         <v>207</v>
       </c>
@@ -5587,7 +5889,9 @@
       <c r="I153" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J153" s="5"/>
+      <c r="J153" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L153" s="5" t="s">
         <v>207</v>
       </c>
@@ -5614,7 +5918,9 @@
       <c r="I154" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="J154" s="5"/>
+      <c r="J154" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L154" s="5" t="s">
         <v>207</v>
       </c>
@@ -5641,7 +5947,9 @@
       <c r="I155" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J155" s="5"/>
+      <c r="J155" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L155" s="5" t="s">
         <v>207</v>
       </c>
@@ -5672,7 +5980,9 @@
       <c r="I156" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J156" s="5"/>
+      <c r="J156" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L156" s="5" t="s">
         <v>207</v>
       </c>
@@ -5699,7 +6009,9 @@
       <c r="I157" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J157" s="5"/>
+      <c r="J157" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L157" s="5" t="s">
         <v>207</v>
       </c>
@@ -5726,7 +6038,9 @@
       <c r="I158" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J158" s="5"/>
+      <c r="J158" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L158" s="5" t="s">
         <v>207</v>
       </c>
@@ -5753,7 +6067,9 @@
       <c r="I159" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J159" s="5"/>
+      <c r="J159" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L159" s="5" t="s">
         <v>207</v>
       </c>
@@ -5784,7 +6100,9 @@
       <c r="I160" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J160" s="5"/>
+      <c r="J160" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L160" s="5" t="s">
         <v>207</v>
       </c>
@@ -5811,7 +6129,9 @@
       <c r="I161" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J161" s="5"/>
+      <c r="J161" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L161" s="5" t="s">
         <v>207</v>
       </c>
@@ -5838,7 +6158,9 @@
       <c r="I162" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J162" s="5"/>
+      <c r="J162" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L162" s="5" t="s">
         <v>207</v>
       </c>
@@ -5865,7 +6187,9 @@
       <c r="I163" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J163" s="5"/>
+      <c r="J163" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L163" s="5" t="s">
         <v>207</v>
       </c>
@@ -5892,7 +6216,9 @@
       <c r="I164" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J164" s="5"/>
+      <c r="J164" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L164" s="5" t="s">
         <v>207</v>
       </c>
@@ -5919,7 +6245,9 @@
       <c r="I165" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J165" s="5"/>
+      <c r="J165" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L165" s="5" t="s">
         <v>207</v>
       </c>
@@ -5946,7 +6274,9 @@
       <c r="I166" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="J166" s="5"/>
+      <c r="J166" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L166" s="5" t="s">
         <v>207</v>
       </c>
@@ -5973,7 +6303,9 @@
       <c r="I167" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J167" s="5"/>
+      <c r="J167" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L167" s="5" t="s">
         <v>207</v>
       </c>
@@ -6000,7 +6332,9 @@
       <c r="I168" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J168" s="5"/>
+      <c r="J168" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L168" s="5" t="s">
         <v>207</v>
       </c>
@@ -6027,7 +6361,9 @@
       <c r="I169" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="J169" s="5"/>
+      <c r="J169" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L169" s="5" t="s">
         <v>207</v>
       </c>
@@ -6054,7 +6390,9 @@
       <c r="I170" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J170" s="5"/>
+      <c r="J170" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L170" s="5" t="s">
         <v>207</v>
       </c>
@@ -6081,7 +6419,9 @@
       <c r="I171" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J171" s="5"/>
+      <c r="J171" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L171" s="5" t="s">
         <v>207</v>
       </c>
@@ -6108,7 +6448,9 @@
       <c r="I172" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J172" s="5"/>
+      <c r="J172" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L172" s="5" t="s">
         <v>207</v>
       </c>
@@ -6135,7 +6477,9 @@
       <c r="I173" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J173" s="5"/>
+      <c r="J173" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L173" s="5" t="s">
         <v>207</v>
       </c>
@@ -6162,7 +6506,9 @@
       <c r="I174" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J174" s="5"/>
+      <c r="J174" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L174" s="5" t="s">
         <v>207</v>
       </c>
@@ -6189,7 +6535,9 @@
       <c r="I175" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J175" s="5"/>
+      <c r="J175" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L175" s="5" t="s">
         <v>207</v>
       </c>
@@ -6216,7 +6564,9 @@
       <c r="I176" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J176" s="5"/>
+      <c r="J176" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L176" s="5" t="s">
         <v>207</v>
       </c>
@@ -6243,7 +6593,9 @@
       <c r="I177" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J177" s="5"/>
+      <c r="J177" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L177" s="5" t="s">
         <v>207</v>
       </c>
@@ -6270,7 +6622,9 @@
       <c r="I178" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J178" s="5"/>
+      <c r="J178" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L178" s="5" t="s">
         <v>207</v>
       </c>
@@ -6297,7 +6651,9 @@
       <c r="I179" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J179" s="5"/>
+      <c r="J179" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L179" s="5" t="s">
         <v>207</v>
       </c>
@@ -6324,7 +6680,9 @@
       <c r="I180" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J180" s="5"/>
+      <c r="J180" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L180" s="5" t="s">
         <v>207</v>
       </c>
@@ -6351,7 +6709,9 @@
       <c r="I181" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J181" s="5"/>
+      <c r="J181" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L181" s="5" t="s">
         <v>207</v>
       </c>
@@ -6378,7 +6738,9 @@
       <c r="I182" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J182" s="5"/>
+      <c r="J182" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L182" s="5" t="s">
         <v>207</v>
       </c>
@@ -6405,7 +6767,9 @@
       <c r="I183" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J183" s="5"/>
+      <c r="J183" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L183" s="5" t="s">
         <v>207</v>
       </c>
@@ -6432,7 +6796,9 @@
       <c r="I184" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J184" s="5"/>
+      <c r="J184" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L184" s="5" t="s">
         <v>207</v>
       </c>
@@ -6459,7 +6825,9 @@
       <c r="I185" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J185" s="5"/>
+      <c r="J185" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L185" s="5" t="s">
         <v>207</v>
       </c>
@@ -6486,7 +6854,9 @@
       <c r="I186" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J186" s="5"/>
+      <c r="J186" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L186" s="5" t="s">
         <v>207</v>
       </c>
@@ -6513,7 +6883,9 @@
       <c r="I187" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J187" s="5"/>
+      <c r="J187" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L187" s="5" t="s">
         <v>207</v>
       </c>
@@ -6540,7 +6912,9 @@
       <c r="I188" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J188" s="5"/>
+      <c r="J188" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L188" s="5" t="s">
         <v>207</v>
       </c>
@@ -6567,7 +6941,9 @@
       <c r="I189" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J189" s="5"/>
+      <c r="J189" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L189" s="5" t="s">
         <v>207</v>
       </c>
@@ -6594,7 +6970,9 @@
       <c r="I190" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J190" s="5"/>
+      <c r="J190" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L190" s="5" t="s">
         <v>207</v>
       </c>
@@ -6621,7 +6999,9 @@
       <c r="I191" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J191" s="5"/>
+      <c r="J191" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L191" s="5" t="s">
         <v>207</v>
       </c>
@@ -6648,7 +7028,9 @@
       <c r="I192" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J192" s="5"/>
+      <c r="J192" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L192" s="5" t="s">
         <v>207</v>
       </c>
@@ -6679,7 +7061,9 @@
       <c r="I193" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J193" s="5"/>
+      <c r="J193" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L193" s="5" t="s">
         <v>207</v>
       </c>
@@ -6706,7 +7090,9 @@
       <c r="I194" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J194" s="5"/>
+      <c r="J194" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L194" s="5" t="s">
         <v>207</v>
       </c>
@@ -6733,7 +7119,9 @@
       <c r="I195" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J195" s="5"/>
+      <c r="J195" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L195" s="5" t="s">
         <v>207</v>
       </c>
@@ -6760,7 +7148,9 @@
       <c r="I196" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J196" s="5"/>
+      <c r="J196" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L196" s="5" t="s">
         <v>207</v>
       </c>
@@ -6787,7 +7177,9 @@
       <c r="I197" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J197" s="5"/>
+      <c r="J197" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L197" s="5" t="s">
         <v>207</v>
       </c>
@@ -6814,7 +7206,9 @@
       <c r="I198" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J198" s="5"/>
+      <c r="J198" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L198" s="5" t="s">
         <v>207</v>
       </c>
@@ -6841,7 +7235,9 @@
       <c r="I199" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J199" s="5"/>
+      <c r="J199" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L199" s="5" t="s">
         <v>207</v>
       </c>
@@ -6868,7 +7264,9 @@
       <c r="I200" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J200" s="5"/>
+      <c r="J200" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L200" s="5" t="s">
         <v>207</v>
       </c>
@@ -6895,7 +7293,9 @@
       <c r="I201" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="J201" s="5"/>
+      <c r="J201" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L201" s="5" t="s">
         <v>207</v>
       </c>
@@ -6922,7 +7322,9 @@
       <c r="I202" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J202" s="5"/>
+      <c r="J202" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L202" s="5" t="s">
         <v>207</v>
       </c>
@@ -6949,7 +7351,9 @@
       <c r="I203" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J203" s="5"/>
+      <c r="J203" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L203" s="5" t="s">
         <v>207</v>
       </c>
@@ -6976,7 +7380,9 @@
       <c r="I204" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J204" s="5"/>
+      <c r="J204" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L204" s="5" t="s">
         <v>207</v>
       </c>
@@ -7007,7 +7413,9 @@
       <c r="I205" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J205" s="5"/>
+      <c r="J205" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L205" s="5" t="s">
         <v>207</v>
       </c>
@@ -7034,7 +7442,9 @@
       <c r="I206" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J206" s="5"/>
+      <c r="J206" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L206" s="5" t="s">
         <v>207</v>
       </c>
@@ -7061,7 +7471,9 @@
       <c r="I207" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J207" s="5"/>
+      <c r="J207" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L207" s="5" t="s">
         <v>207</v>
       </c>
@@ -7088,7 +7500,9 @@
       <c r="I208" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J208" s="5"/>
+      <c r="J208" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L208" s="5" t="s">
         <v>207</v>
       </c>
@@ -7115,7 +7529,9 @@
       <c r="I209" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J209" s="5"/>
+      <c r="J209" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L209" s="5" t="s">
         <v>207</v>
       </c>
@@ -7142,7 +7558,9 @@
       <c r="I210" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J210" s="5"/>
+      <c r="J210" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L210" s="5" t="s">
         <v>207</v>
       </c>
@@ -7169,7 +7587,9 @@
       <c r="I211" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J211" s="5"/>
+      <c r="J211" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L211" s="5" t="s">
         <v>207</v>
       </c>
@@ -7196,7 +7616,9 @@
       <c r="I212" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J212" s="5"/>
+      <c r="J212" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L212" s="5" t="s">
         <v>207</v>
       </c>
@@ -7223,7 +7645,9 @@
       <c r="I213" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J213" s="5"/>
+      <c r="J213" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L213" s="5" t="s">
         <v>207</v>
       </c>
@@ -7250,7 +7674,9 @@
       <c r="I214" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J214" s="5"/>
+      <c r="J214" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L214" s="5" t="s">
         <v>207</v>
       </c>
@@ -7277,7 +7703,9 @@
       <c r="I215" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J215" s="5"/>
+      <c r="J215" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L215" s="5" t="s">
         <v>207</v>
       </c>
@@ -7304,7 +7732,9 @@
       <c r="I216" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J216" s="5"/>
+      <c r="J216" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L216" s="5" t="s">
         <v>207</v>
       </c>
@@ -7335,7 +7765,9 @@
       <c r="I217" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J217" s="5"/>
+      <c r="J217" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L217" s="5" t="s">
         <v>207</v>
       </c>
@@ -7362,7 +7794,9 @@
       <c r="I218" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J218" s="5"/>
+      <c r="J218" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L218" s="5" t="s">
         <v>207</v>
       </c>
@@ -7389,7 +7823,9 @@
       <c r="I219" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J219" s="5"/>
+      <c r="J219" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L219" s="5" t="s">
         <v>207</v>
       </c>
@@ -7416,7 +7852,9 @@
       <c r="I220" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J220" s="5"/>
+      <c r="J220" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L220" s="5" t="s">
         <v>207</v>
       </c>
@@ -7443,7 +7881,9 @@
       <c r="I221" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J221" s="5"/>
+      <c r="J221" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L221" s="5" t="s">
         <v>207</v>
       </c>
@@ -7470,7 +7910,9 @@
       <c r="I222" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J222" s="5"/>
+      <c r="J222" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L222" s="5" t="s">
         <v>207</v>
       </c>
@@ -7497,7 +7939,9 @@
       <c r="I223" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J223" s="5"/>
+      <c r="J223" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L223" s="5" t="s">
         <v>207</v>
       </c>
@@ -7524,7 +7968,9 @@
       <c r="I224" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J224" s="5"/>
+      <c r="J224" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L224" s="5" t="s">
         <v>207</v>
       </c>
@@ -7551,7 +7997,9 @@
       <c r="I225" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J225" s="5"/>
+      <c r="J225" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L225" s="5" t="s">
         <v>207</v>
       </c>
@@ -7582,7 +8030,9 @@
       <c r="I226" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J226" s="5"/>
+      <c r="J226" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L226" s="5" t="s">
         <v>207</v>
       </c>
@@ -7609,7 +8059,9 @@
       <c r="I227" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J227" s="5"/>
+      <c r="J227" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L227" s="5" t="s">
         <v>207</v>
       </c>
@@ -7636,7 +8088,9 @@
       <c r="I228" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J228" s="5"/>
+      <c r="J228" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L228" s="5" t="s">
         <v>207</v>
       </c>
@@ -7663,7 +8117,9 @@
       <c r="I229" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J229" s="5"/>
+      <c r="J229" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L229" s="5" t="s">
         <v>207</v>
       </c>
@@ -7690,7 +8146,9 @@
       <c r="I230" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="J230" s="5"/>
+      <c r="J230" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L230" s="5" t="s">
         <v>207</v>
       </c>
@@ -7717,7 +8175,9 @@
       <c r="I231" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J231" s="5"/>
+      <c r="J231" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L231" s="5" t="s">
         <v>207</v>
       </c>
@@ -7744,7 +8204,9 @@
       <c r="I232" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J232" s="5"/>
+      <c r="J232" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L232" s="5" t="s">
         <v>207</v>
       </c>
@@ -7771,7 +8233,9 @@
       <c r="I233" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J233" s="5"/>
+      <c r="J233" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L233" s="5" t="s">
         <v>207</v>
       </c>
@@ -7798,7 +8262,9 @@
       <c r="I234" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J234" s="5"/>
+      <c r="J234" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L234" s="5" t="s">
         <v>207</v>
       </c>
@@ -7825,7 +8291,9 @@
       <c r="I235" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J235" s="5"/>
+      <c r="J235" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L235" s="5" t="s">
         <v>207</v>
       </c>
@@ -7852,7 +8320,9 @@
       <c r="I236" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J236" s="5"/>
+      <c r="J236" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L236" s="5" t="s">
         <v>207</v>
       </c>
@@ -7879,7 +8349,9 @@
       <c r="I237" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J237" s="5"/>
+      <c r="J237" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L237" s="5" t="s">
         <v>207</v>
       </c>
@@ -7909,7 +8381,9 @@
       <c r="I238" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="J238" s="5"/>
+      <c r="J238" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L238" s="5" t="s">
         <v>207</v>
       </c>
@@ -7936,7 +8410,9 @@
       <c r="I239" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J239" s="5"/>
+      <c r="J239" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L239" s="5" t="s">
         <v>207</v>
       </c>
@@ -7963,7 +8439,9 @@
       <c r="I240" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="J240" s="5"/>
+      <c r="J240" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L240" s="5" t="s">
         <v>207</v>
       </c>
@@ -7990,7 +8468,9 @@
       <c r="I241" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J241" s="5"/>
+      <c r="J241" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L241" s="5" t="s">
         <v>207</v>
       </c>
@@ -8017,7 +8497,9 @@
       <c r="I242" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J242" s="5"/>
+      <c r="J242" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L242" s="5" t="s">
         <v>207</v>
       </c>
@@ -8047,7 +8529,9 @@
       <c r="I243" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="J243" s="5"/>
+      <c r="J243" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L243" s="5" t="s">
         <v>207</v>
       </c>
@@ -8074,7 +8558,9 @@
       <c r="I244" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="J244" s="5"/>
+      <c r="J244" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L244" s="5" t="s">
         <v>207</v>
       </c>
@@ -8101,7 +8587,9 @@
       <c r="I245" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J245" s="5"/>
+      <c r="J245" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L245" s="5" t="s">
         <v>207</v>
       </c>
@@ -8128,7 +8616,9 @@
       <c r="I246" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J246" s="5"/>
+      <c r="J246" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L246" s="5" t="s">
         <v>207</v>
       </c>
@@ -8159,7 +8649,9 @@
       <c r="I247" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="J247" s="5"/>
+      <c r="J247" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L247" s="5" t="s">
         <v>207</v>
       </c>
@@ -8187,7 +8679,9 @@
       <c r="I248" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J248" s="5"/>
+      <c r="J248" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L248" s="5" t="s">
         <v>207</v>
       </c>
@@ -8217,7 +8711,9 @@
       <c r="I249" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J249" s="5"/>
+      <c r="J249" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L249" s="5" t="s">
         <v>207</v>
       </c>
@@ -8244,7 +8740,9 @@
       <c r="I250" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="J250" s="5"/>
+      <c r="J250" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L250" s="5" t="s">
         <v>207</v>
       </c>
@@ -8271,7 +8769,9 @@
       <c r="I251" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J251" s="5"/>
+      <c r="J251" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L251" s="5" t="s">
         <v>207</v>
       </c>
@@ -8298,7 +8798,9 @@
       <c r="I252" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J252" s="5"/>
+      <c r="J252" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L252" s="5" t="s">
         <v>207</v>
       </c>
@@ -8325,7 +8827,9 @@
       <c r="I253" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J253" s="5"/>
+      <c r="J253" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L253" s="5" t="s">
         <v>207</v>
       </c>
@@ -8352,7 +8856,9 @@
       <c r="I254" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J254" s="5"/>
+      <c r="J254" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L254" s="5" t="s">
         <v>207</v>
       </c>
@@ -8379,7 +8885,9 @@
       <c r="I255" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="J255" s="5"/>
+      <c r="J255" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L255" s="5" t="s">
         <v>207</v>
       </c>
@@ -8406,7 +8914,9 @@
       <c r="I256" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J256" s="5"/>
+      <c r="J256" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L256" s="5" t="s">
         <v>207</v>
       </c>
@@ -8433,7 +8943,9 @@
       <c r="I257" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J257" s="5"/>
+      <c r="J257" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L257" s="5" t="s">
         <v>207</v>
       </c>
@@ -8460,7 +8972,9 @@
       <c r="I258" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J258" s="5"/>
+      <c r="J258" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L258" s="5" t="s">
         <v>207</v>
       </c>
@@ -8493,7 +9007,9 @@
       <c r="I259" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="J259" s="11"/>
+      <c r="J259" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K259" s="10"/>
       <c r="L259" s="12" t="s">
         <v>213</v>
@@ -8536,7 +9052,9 @@
       <c r="I260" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="J260" s="11"/>
+      <c r="J260" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K260" s="11" t="s">
         <v>216</v>
       </c>
@@ -8587,7 +9105,9 @@
       <c r="I261" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="J261" s="11"/>
+      <c r="J261" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K261" s="10"/>
       <c r="L261" s="12" t="s">
         <v>213</v>
@@ -8630,7 +9150,9 @@
       <c r="I262" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J262" s="11"/>
+      <c r="J262" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K262" s="10"/>
       <c r="L262" s="12" t="s">
         <v>213</v>
@@ -8679,7 +9201,9 @@
       <c r="I263" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="J263" s="11"/>
+      <c r="J263" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K263" s="10"/>
       <c r="L263" s="12" t="s">
         <v>213</v>
@@ -8720,7 +9244,9 @@
       <c r="I264" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="J264" s="11"/>
+      <c r="J264" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K264" s="10"/>
       <c r="L264" s="12" t="s">
         <v>213</v>
@@ -8761,7 +9287,9 @@
       <c r="I265" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J265" s="11"/>
+      <c r="J265" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K265" s="10"/>
       <c r="L265" s="12" t="s">
         <v>213</v>
@@ -8808,7 +9336,9 @@
       <c r="I266" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J266" s="11"/>
+      <c r="J266" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K266" s="10"/>
       <c r="L266" s="12" t="s">
         <v>213</v>
@@ -8855,7 +9385,9 @@
       <c r="I267" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="J267" s="11"/>
+      <c r="J267" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K267" s="10"/>
       <c r="L267" s="12" t="s">
         <v>213</v>
@@ -8892,7 +9424,9 @@
       <c r="I268" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J268" s="5"/>
+      <c r="J268" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L268" s="5" t="s">
         <v>207</v>
       </c>
@@ -8919,7 +9453,9 @@
       <c r="I269" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J269" s="5"/>
+      <c r="J269" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L269" s="5" t="s">
         <v>207</v>
       </c>
@@ -8946,7 +9482,9 @@
       <c r="I270" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J270" s="5"/>
+      <c r="J270" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L270" s="5" t="s">
         <v>207</v>
       </c>
@@ -8973,7 +9511,9 @@
       <c r="I271" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="J271" s="5"/>
+      <c r="J271" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L271" s="5" t="s">
         <v>207</v>
       </c>
@@ -9000,7 +9540,9 @@
       <c r="I272" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J272" s="5"/>
+      <c r="J272" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L272" s="5" t="s">
         <v>207</v>
       </c>
@@ -9030,7 +9572,9 @@
       <c r="I273" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="J273" s="5"/>
+      <c r="J273" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L273" s="5" t="s">
         <v>207</v>
       </c>
@@ -9061,7 +9605,9 @@
       <c r="I274" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="J274" s="11"/>
+      <c r="J274" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K274" s="10"/>
       <c r="L274" s="12" t="s">
         <v>213</v>
@@ -9102,7 +9648,9 @@
       <c r="I275" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J275" s="11"/>
+      <c r="J275" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K275" s="10"/>
       <c r="L275" s="12" t="s">
         <v>213</v>
@@ -9149,7 +9697,9 @@
       <c r="I276" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J276" s="11"/>
+      <c r="J276" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K276" s="10"/>
       <c r="L276" s="12" t="s">
         <v>213</v>
@@ -9196,7 +9746,9 @@
       <c r="I277" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="J277" s="11"/>
+      <c r="J277" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K277" s="10"/>
       <c r="L277" s="12" t="s">
         <v>213</v>
@@ -9233,7 +9785,9 @@
       <c r="I278" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J278" s="5"/>
+      <c r="J278" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L278" s="5" t="s">
         <v>207</v>
       </c>
@@ -9263,7 +9817,9 @@
       <c r="I279" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J279" s="5"/>
+      <c r="J279" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L279" s="5" t="s">
         <v>207</v>
       </c>
@@ -9302,7 +9858,9 @@
       <c r="I280" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J280" s="5"/>
+      <c r="J280" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L280" s="5" t="s">
         <v>207</v>
       </c>
@@ -9341,7 +9899,9 @@
       <c r="I281" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="J281" s="5"/>
+      <c r="J281" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L281" s="5" t="s">
         <v>207</v>
       </c>
@@ -9372,7 +9932,9 @@
       <c r="I282" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="J282" s="11"/>
+      <c r="J282" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K282" s="10"/>
       <c r="L282" s="12" t="s">
         <v>213</v>
@@ -9413,7 +9975,9 @@
       <c r="I283" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="J283" s="11"/>
+      <c r="J283" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K283" s="10"/>
       <c r="L283" s="12" t="s">
         <v>213</v>
@@ -9454,7 +10018,9 @@
       <c r="I284" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="J284" s="11"/>
+      <c r="J284" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K284" s="11" t="s">
         <v>243</v>
       </c>
@@ -9497,7 +10063,9 @@
       <c r="I285" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="J285" s="11"/>
+      <c r="J285" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K285" s="10"/>
       <c r="L285" s="12" t="s">
         <v>213</v>
@@ -9538,7 +10106,9 @@
       <c r="I286" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J286" s="11"/>
+      <c r="J286" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K286" s="10"/>
       <c r="L286" s="12" t="s">
         <v>213</v>
@@ -9587,7 +10157,9 @@
       <c r="I287" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J287" s="11"/>
+      <c r="J287" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L287" s="12" t="s">
         <v>213</v>
       </c>
@@ -9625,7 +10197,9 @@
       <c r="I288" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="J288" s="11"/>
+      <c r="J288" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L288" s="12" t="s">
         <v>213</v>
       </c>
@@ -9656,7 +10230,9 @@
       <c r="I289" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="J289" s="5"/>
+      <c r="J289" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K289"/>
       <c r="L289" s="5" t="s">
         <v>207</v>
@@ -9695,7 +10271,9 @@
       <c r="I290" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="J290" s="5"/>
+      <c r="J290" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K290"/>
       <c r="L290" s="5" t="s">
         <v>207</v>
@@ -9734,7 +10312,9 @@
       <c r="I291" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J291" s="5"/>
+      <c r="J291" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K291"/>
       <c r="L291" s="5" t="s">
         <v>207</v>
@@ -9773,7 +10353,9 @@
       <c r="I292" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J292" s="5"/>
+      <c r="J292" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K292"/>
       <c r="L292" s="5" t="s">
         <v>207</v>
@@ -9814,7 +10396,9 @@
       <c r="I293" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="J293" s="5"/>
+      <c r="J293" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K293"/>
       <c r="L293" s="5" t="s">
         <v>207</v>
@@ -9857,7 +10441,9 @@
       <c r="I294" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="J294" s="11"/>
+      <c r="J294" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L294" s="12" t="s">
         <v>213</v>
       </c>
@@ -9889,7 +10475,9 @@
       <c r="I295" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J295" s="11"/>
+      <c r="J295" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L295" s="12" t="s">
         <v>213</v>
       </c>
@@ -9925,7 +10513,9 @@
       <c r="I296" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J296" s="11"/>
+      <c r="J296" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L296" s="12" t="s">
         <v>213</v>
       </c>
@@ -9960,7 +10550,9 @@
       <c r="I297" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="J297" s="11"/>
+      <c r="J297" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L297" s="12" t="s">
         <v>213</v>
       </c>
@@ -9991,7 +10583,9 @@
       <c r="I298" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J298" s="5"/>
+      <c r="J298" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K298"/>
       <c r="L298" s="5" t="s">
         <v>207</v>
@@ -10030,7 +10624,9 @@
       <c r="I299" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J299" s="5"/>
+      <c r="J299" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K299"/>
       <c r="L299" s="5" t="s">
         <v>207</v>
@@ -10069,7 +10665,9 @@
       <c r="I300" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J300" s="5"/>
+      <c r="J300" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K300"/>
       <c r="L300" s="5" t="s">
         <v>207</v>
@@ -10110,7 +10708,9 @@
       <c r="I301" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J301" s="5"/>
+      <c r="J301" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K301"/>
       <c r="L301" s="5" t="s">
         <v>207</v>
@@ -10190,7 +10790,9 @@
       <c r="I303" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J303" s="5"/>
+      <c r="J303" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K303"/>
       <c r="L303" s="5" t="s">
         <v>207</v>
@@ -10229,7 +10831,9 @@
       <c r="I304" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J304" s="5"/>
+      <c r="J304" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K304"/>
       <c r="L304" s="5" t="s">
         <v>207</v>
@@ -10268,7 +10872,9 @@
       <c r="I305" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J305" s="5"/>
+      <c r="J305" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K305"/>
       <c r="L305" s="5" t="s">
         <v>207</v>
@@ -10309,7 +10915,9 @@
       <c r="I306" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J306" s="5"/>
+      <c r="J306" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K306"/>
       <c r="L306" s="5" t="s">
         <v>207</v>
@@ -10349,7 +10957,9 @@
       <c r="I307" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="J307" s="11"/>
+      <c r="J307" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L307" s="12" t="s">
         <v>213</v>
       </c>
@@ -10381,7 +10991,9 @@
       <c r="I308" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J308" s="11"/>
+      <c r="J308" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L308" s="12" t="s">
         <v>213</v>
       </c>
@@ -10417,7 +11029,9 @@
       <c r="I309" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="J309" s="11"/>
+      <c r="J309" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L309" s="12" t="s">
         <v>213</v>
       </c>
@@ -10452,7 +11066,9 @@
       <c r="I310" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="J310" s="11"/>
+      <c r="J310" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="L310" s="12" t="s">
         <v>213</v>
       </c>
@@ -10483,7 +11099,9 @@
       <c r="I311" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J311" s="5"/>
+      <c r="J311" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K311"/>
       <c r="L311" s="5" t="s">
         <v>207</v>
@@ -10522,7 +11140,9 @@
       <c r="I312" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J312" s="5"/>
+      <c r="J312" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K312"/>
       <c r="L312" s="5" t="s">
         <v>207</v>
@@ -10561,7 +11181,9 @@
       <c r="I313" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J313" s="5"/>
+      <c r="J313" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K313"/>
       <c r="L313" s="5" t="s">
         <v>207</v>
@@ -10602,7 +11224,9 @@
       <c r="I314" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J314" s="5"/>
+      <c r="J314" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="K314"/>
       <c r="L314" s="5" t="s">
         <v>207</v>
@@ -10617,7 +11241,7 @@
       <c r="T314"/>
       <c r="U314"/>
     </row>
-    <row r="315" spans="1:21" s="10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:21" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A315" s="10" t="s">
         <v>27</v>
       </c>
@@ -10646,7 +11270,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="316" spans="1:21" s="10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:21" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A316" s="10" t="s">
         <v>27</v>
       </c>
@@ -10675,7 +11299,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="317" spans="1:21" s="10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:21" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A317" s="10" t="s">
         <v>27</v>
       </c>
@@ -10704,7 +11328,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="318" spans="1:21" s="10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:21" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A318" s="10" t="s">
         <v>27</v>
       </c>
@@ -10733,7 +11357,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="319" spans="1:21" s="10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:21" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A319" s="10" t="s">
         <v>27</v>
       </c>
@@ -10762,7 +11386,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="320" spans="1:21" s="10" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:21" s="10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A320" s="10" t="s">
         <v>27</v>
       </c>
@@ -12881,8 +13505,8 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="J232" sqref="J232:J235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18728,7 +19352,9 @@
       <c r="I197" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="J197" s="11"/>
+      <c r="J197" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K197" s="10"/>
       <c r="L197" s="12" t="s">
         <v>256</v>
@@ -18767,7 +19393,9 @@
       <c r="I198" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J198" s="11"/>
+      <c r="J198" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K198" s="10"/>
       <c r="L198" s="12" t="s">
         <v>256</v>
@@ -18806,7 +19434,9 @@
       <c r="I199" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J199" s="11"/>
+      <c r="J199" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K199" s="10"/>
       <c r="L199" s="12" t="s">
         <v>256</v>
@@ -18847,7 +19477,9 @@
       <c r="I200" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="J200" s="11"/>
+      <c r="J200" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K200" s="10"/>
       <c r="L200" s="12" t="s">
         <v>256</v>
@@ -18973,7 +19605,9 @@
       <c r="I204" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J204" s="11"/>
+      <c r="J204" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K204" s="10"/>
       <c r="L204" s="12" t="s">
         <v>256</v>
@@ -19012,7 +19646,9 @@
       <c r="I205" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J205" s="11"/>
+      <c r="J205" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K205" s="10"/>
       <c r="L205" s="12" t="s">
         <v>256</v>
@@ -19053,7 +19689,9 @@
       <c r="I206" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="J206" s="11"/>
+      <c r="J206" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K206" s="10"/>
       <c r="L206" s="12" t="s">
         <v>256</v>
@@ -19179,7 +19817,9 @@
       <c r="I210" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J210" s="11"/>
+      <c r="J210" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K210" s="10"/>
       <c r="L210" s="12" t="s">
         <v>256</v>
@@ -19220,7 +19860,9 @@
       <c r="I211" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J211" s="11"/>
+      <c r="J211" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K211" s="10"/>
       <c r="L211" s="12" t="s">
         <v>256</v>
@@ -19267,7 +19909,9 @@
       <c r="I212" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="J212" s="11"/>
+      <c r="J212" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K212" s="10"/>
       <c r="L212" s="12" t="s">
         <v>256</v>
@@ -19393,7 +20037,9 @@
       <c r="I216" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="J216" s="11"/>
+      <c r="J216" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K216" s="10"/>
       <c r="L216" s="12" t="s">
         <v>256</v>
@@ -19432,7 +20078,9 @@
       <c r="I217" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="J217" s="11"/>
+      <c r="J217" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K217" s="10"/>
       <c r="L217" s="12" t="s">
         <v>256</v>
@@ -19471,7 +20119,9 @@
       <c r="I218" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J218" s="11"/>
+      <c r="J218" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K218" s="10"/>
       <c r="L218" s="12" t="s">
         <v>256</v>
@@ -19510,7 +20160,9 @@
       <c r="I219" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J219" s="11"/>
+      <c r="J219" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K219" s="10"/>
       <c r="L219" s="12" t="s">
         <v>256</v>
@@ -19551,7 +20203,9 @@
       <c r="I220" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="J220" s="11"/>
+      <c r="J220" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K220" s="10"/>
       <c r="L220" s="12" t="s">
         <v>256</v>
@@ -19677,7 +20331,9 @@
       <c r="I224" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J224" s="11"/>
+      <c r="J224" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K224" s="10"/>
       <c r="L224" s="12" t="s">
         <v>256</v>
@@ -19716,7 +20372,9 @@
       <c r="I225" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J225" s="11"/>
+      <c r="J225" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K225" s="10"/>
       <c r="L225" s="12" t="s">
         <v>256</v>
@@ -19755,7 +20413,9 @@
       <c r="I226" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="J226" s="11"/>
+      <c r="J226" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K226" s="10"/>
       <c r="L226" s="12" t="s">
         <v>256</v>
@@ -19968,7 +20628,9 @@
       <c r="I233" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J233" s="11"/>
+      <c r="J233" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K233" s="10"/>
       <c r="L233" s="12" t="s">
         <v>256</v>
@@ -20007,7 +20669,9 @@
       <c r="I234" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="J234" s="11"/>
+      <c r="J234" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K234" s="10"/>
       <c r="L234" s="12" t="s">
         <v>256</v>
@@ -20046,7 +20710,9 @@
       <c r="I235" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="J235" s="11"/>
+      <c r="J235" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="K235" s="10"/>
       <c r="L235" s="12" t="s">
         <v>256</v>

</xml_diff>